<commit_message>
added code for Index and composite index.
</commit_message>
<xml_diff>
--- a/DP-420-COSMOS-DB.xlsx
+++ b/DP-420-COSMOS-DB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Projects\CosmosDBEmployeeManagementAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7870443A-BB5B-4EFE-B95A-6517E0D58071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523CAA15-25D9-4DC9-968A-868B3F8546D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Get started with Azure Cosmos DB for NoSQL</t>
   </si>
@@ -84,6 +84,23 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>1.Built in function
+2.Cross product join</t>
+  </si>
+  <si>
+    <t>Define and implement an indexing strategy for Azure Cosmos DB for NoSQL</t>
+  </si>
+  <si>
+    <t>1.Default Indexing Policy.
+2.Custom Indexing Policy.
+3.Strategy 1 - Include all and Exclude specific path
+4.Strategy 2 - Exclude all and Include specific path
+5.Composite Index.</t>
+  </si>
+  <si>
+    <t>Integrate Azure Cosmos DB for NoSQL with Azure services</t>
   </si>
 </sst>
 </file>
@@ -422,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
@@ -497,12 +514,14 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3">
         <v>45437</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="3">
+        <v>45436</v>
+      </c>
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
@@ -515,7 +534,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <v>45435</v>
@@ -530,15 +549,55 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5">
         <v>45437</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45438</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45441</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45444</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Index Metrics and Cache
</commit_message>
<xml_diff>
--- a/DP-420-COSMOS-DB.xlsx
+++ b/DP-420-COSMOS-DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Projects\CosmosDBEmployeeManagementAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23349FA-CAFC-468C-A207-0D28E94CB745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE5566B-F95C-4864-99BF-F469E9517839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Get started with Azure Cosmos DB for NoSQL</t>
   </si>
@@ -120,6 +120,28 @@
   </si>
   <si>
     <t>Design and implement a replication strategy for Azure Cosmos DB for NoSQL</t>
+  </si>
+  <si>
+    <t>1.Data replication across globe.
+2.Cost of data replication.(no of RU's/region* number of regions)
+3.Automatic failover
+4.Manual failover.
+5.Configure Consistancy model.
+6.Configure multi region writes.</t>
+  </si>
+  <si>
+    <t>Done.Theory.</t>
+  </si>
+  <si>
+    <t>Optimize query and operation performance in Azure Cosmos DB for NoSQL</t>
+  </si>
+  <si>
+    <t>1.Custom Index Policy
+2.Read heavy Application.
+3.Write Heavy Application.
+4.Index Metrics (suggest if need any index for query)
+5.Measure Query cost.
+6.Integrated Cache (client’s consistency level must be set to session or eventual)</t>
   </si>
 </sst>
 </file>
@@ -488,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,10 +699,10 @@
         <v>22</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
@@ -690,17 +712,33 @@
       <c r="C10" s="7">
         <v>45446</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="D10" s="7">
+        <v>45446</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="10">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7">
+        <v>45447</v>
+      </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
+      <c r="E11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>

</xml_diff>

<commit_message>
added SP, UDF and Trigger controller.
</commit_message>
<xml_diff>
--- a/DP-420-COSMOS-DB.xlsx
+++ b/DP-420-COSMOS-DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Projects\CosmosDBEmployeeManagementAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE5566B-F95C-4864-99BF-F469E9517839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF425CB-F65A-4E1C-A4AB-8AA08D4595EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Get started with Azure Cosmos DB for NoSQL</t>
   </si>
@@ -142,6 +142,21 @@
 4.Index Metrics (suggest if need any index for query)
 5.Measure Query cost.
 6.Integrated Cache (client’s consistency level must be set to session or eventual)</t>
+  </si>
+  <si>
+    <t>Create server-side programming constructs in Azure Cosmos DB for NoSQL</t>
+  </si>
+  <si>
+    <t>1.Stored Proc in Javascript Language.
+2.Create Stored Proc using .Net SDK.
+3.User Defined Function.
+(
+1.DFs can only be called from inside queries.
+2.UDFs do not have access to the context object and are meant to be used as compute-only code.
+3.UDF's takes in one or more scalar input[s] and then returns a scalar value.
+)
+4.Trigger(PRE and POST).
+5.Create UDF's and Triggers with SDK.</t>
   </si>
 </sst>
 </file>
@@ -510,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,12 +771,20 @@
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+    <row r="14" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="10">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7">
+        <v>45464</v>
+      </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="F14" s="10"/>
     </row>
   </sheetData>

</xml_diff>